<commit_message>
Planning - mise en italique des "bonus"
</commit_message>
<xml_diff>
--- a/planning_stage.xlsx
+++ b/planning_stage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>SEMAINE</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Export (fonctionnel) de templates (par galaxie) et instances (par template) -&gt; CSV</t>
   </si>
   <si>
-    <t>Export (fonctionnel) de templates (par galaxie) et instances (par template) -&gt; XLSX</t>
-  </si>
-  <si>
     <t>Contrôleur d'import avec liste de validation + bouton retrait d'éléments</t>
   </si>
   <si>
@@ -178,13 +175,16 @@
   </si>
   <si>
     <t>? (Raccourcis clavier (Ctrl+…) pour : recherche (F), refresh (U), layout (L))</t>
+  </si>
+  <si>
+    <t>Export (fonctionnel) de templates (par galaxie) et instances (par template) -&gt; CSV/XLSX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +238,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -286,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -307,6 +315,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,16 +623,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="76.42578125" customWidth="1"/>
+    <col min="3" max="3" width="77.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -641,7 +651,7 @@
       <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="14">
         <v>42429</v>
       </c>
       <c r="B2" s="4"/>
@@ -736,63 +746,63 @@
         <v>42436</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -806,35 +816,35 @@
         <v>42443</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
+      <c r="C26" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="3" t="s">
-        <v>42</v>
+      <c r="C27" s="15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -856,42 +866,42 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="4"/>
       <c r="C37" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -918,147 +928,147 @@
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+      <c r="A42" s="6"/>
       <c r="B42" s="4"/>
       <c r="C42" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="4"/>
       <c r="C43" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="3" t="s">
-        <v>10</v>
+      <c r="C44" s="13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A45" s="7"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
+      <c r="A46" s="5">
+        <v>42464</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>42464</v>
-      </c>
+      <c r="A47" s="5"/>
       <c r="B47" s="4"/>
       <c r="C47" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="3" t="s">
+      <c r="A48" s="7"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>42471</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="10"/>
-    </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
-        <v>42471</v>
-      </c>
+      <c r="A50" s="6"/>
       <c r="B50" s="4"/>
       <c r="C50" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="10"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>42478</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="10"/>
-    </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
-        <v>42478</v>
-      </c>
+      <c r="A53" s="6"/>
       <c r="B53" s="4"/>
       <c r="C53" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="3" t="s">
+      <c r="A54" s="7"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="10"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>42485</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="10"/>
-    </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
-        <v>42485</v>
-      </c>
+      <c r="A56" s="6"/>
       <c r="B56" s="4"/>
-      <c r="C56" s="3" t="s">
-        <v>47</v>
+      <c r="C56" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="4"/>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="10"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>42492</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-    </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
-        <v>42492</v>
-      </c>
+      <c r="A60" s="6"/>
       <c r="B60" s="4"/>
-      <c r="C60" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="C60" s="13"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="4"/>
-      <c r="C61" s="3"/>
+      <c r="C61" s="13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
@@ -1078,23 +1088,16 @@
       <c r="A64" s="6"/>
       <c r="B64" s="4"/>
       <c r="C64" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="A65" s="7"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="10"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="10"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+      <c r="A66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Images, sources, planning (début semaine 7/3)
</commit_message>
<xml_diff>
--- a/planning_stage.xlsx
+++ b/planning_stage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="23715" windowHeight="14370"/>
+    <workbookView xWindow="135" yWindow="120" windowWidth="23715" windowHeight="14325"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>SEMAINE</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Filtrage de liste (selon la valeur partielle d'une colonne, insensible à la casse)</t>
   </si>
   <si>
-    <t>Gestion de tâches asynchrones interruptibles/remplaçables</t>
-  </si>
-  <si>
     <t>Récup async interruptible d'instances de sélection + selon paramètres desc</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Barre de statut mise à jour selon instances listées et sélection</t>
   </si>
   <si>
-    <t>Synchronisation des sélections d'arbres (depuis actif vers masqué ou l'inverse)</t>
-  </si>
-  <si>
     <t>Boite de recherche (plusieurs colonnes selon config)</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Historique de recherche global avec longueur max (configurable) + fct changer max</t>
   </si>
   <si>
-    <t>Navigation dans l'arbre actif selon sélection de recherche (templ ou parent d'inst)</t>
-  </si>
-  <si>
     <t>Contrôleur d'export avec liste de sélection</t>
   </si>
   <si>
@@ -114,9 +105,6 @@
     <t>Contrôleur d'import avec liste de validation + bouton retrait d'éléments</t>
   </si>
   <si>
-    <t>Import (fonctionnel) d'instances (par template) depuis CSV et XLSX vers liste</t>
-  </si>
-  <si>
     <t>Liste validation affiche erreurs (ou boite de dialogue les mentionne)</t>
   </si>
   <si>
@@ -153,9 +141,6 @@
     <t>Système de chargement/sauvegarde de snapshot d'état des arbres</t>
   </si>
   <si>
-    <t>Ajout export structurel pour comparaison (tout ou par critère) -&gt; *.txt</t>
-  </si>
-  <si>
     <t>Amélioration gestion de tâches et file d'attente</t>
   </si>
   <si>
@@ -168,9 +153,6 @@
     <t>? (Raccourcis clavier (Ctrl+…) pour : recherche (F), refresh (U), layout (L))</t>
   </si>
   <si>
-    <t>Export (fonctionnel) de templates (par galaxie) et instances (par template) -&gt; CSV/XLSX</t>
-  </si>
-  <si>
     <t>Export (fonctionnel) de templates et instances : débug</t>
   </si>
   <si>
@@ -183,14 +165,47 @@
     <t>Navigation depuis recherche: additionnée ou remplacement sélection</t>
   </si>
   <si>
-    <t>Divers : stats (hôte,gal.,nb templ.) + nb inst. chargées + compter nb total (sauf vues, …)</t>
+    <t>Import (fonctionnel) : debug</t>
+  </si>
+  <si>
+    <t>Optimisation récupération et vitesse affichage (de 16 sec à 1 sec)</t>
+  </si>
+  <si>
+    <t>Gestion de tâches asynchrones interruptibles/remplaçables + gestion annulation</t>
+  </si>
+  <si>
+    <t>Boite de progression avec titre, numéro d'étape, croix d'annulation</t>
+  </si>
+  <si>
+    <t>Ajout export CSV à la manière d'ArchestrA</t>
+  </si>
+  <si>
+    <t>Export (fonctionnel) de templates (par galaxie) et instances (par template) -&gt; XLSX</t>
+  </si>
+  <si>
+    <t>Import (fonctionnel) d'instances (par template) ou tmpl depuis XLSX vers liste</t>
+  </si>
+  <si>
+    <t>Double clic résultats recherche : navigation avec remplacement</t>
+  </si>
+  <si>
+    <t>Navigation dans l'arbre actif selon sélection de recherche (templ ou parent d'inst) + liste</t>
+  </si>
+  <si>
+    <t>Synchronisation des sélections d'arbres (depuis actif vers masqué)</t>
+  </si>
+  <si>
+    <t>? (Divers : stats (hôte,galax,nb tmpl) + nb inst chargées + nb total (sauf vues, …))</t>
+  </si>
+  <si>
+    <t>UI Contrôleur d'export avec liste de sélection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +267,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -300,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -323,6 +353,8 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,6 +369,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -629,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +739,7 @@
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -748,333 +783,333 @@
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="17">
         <v>42436</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="15" t="s">
-        <v>19</v>
+      <c r="C15" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="15" t="s">
-        <v>20</v>
+      <c r="C16" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="15" t="s">
-        <v>22</v>
+      <c r="C17" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="15" t="s">
-        <v>24</v>
+      <c r="C18" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="15" t="s">
-        <v>26</v>
+      <c r="C19" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="15" t="s">
-        <v>25</v>
+      <c r="C20" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="15" t="s">
-        <v>27</v>
+      <c r="C21" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="13" t="s">
-        <v>54</v>
+      <c r="C22" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="13" t="s">
-        <v>23</v>
+      <c r="C23" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="13" t="s">
-        <v>55</v>
+      <c r="C24" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>42443</v>
-      </c>
+      <c r="A26" s="6"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="15" t="s">
-        <v>28</v>
+      <c r="C26" s="16" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="A28" s="7"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="5">
+        <v>42443</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="C29" s="15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="5"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="3" t="s">
-        <v>50</v>
+      <c r="C30" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="13" t="s">
-        <v>30</v>
+      <c r="C31" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="15" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>42450</v>
-      </c>
+      <c r="A33" s="6"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="A34" s="6"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="3" t="s">
-        <v>31</v>
+      <c r="C34" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="A35" s="7"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
+      <c r="A36" s="5">
+        <v>42450</v>
+      </c>
       <c r="B36" s="4"/>
       <c r="C36" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="5"/>
       <c r="B37" s="4"/>
       <c r="C37" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+      <c r="A38" s="5"/>
       <c r="B38" s="4"/>
       <c r="C38" s="3" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>42457</v>
-      </c>
+      <c r="A40" s="6"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
+      <c r="A41" s="6"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="13" t="s">
-        <v>52</v>
-      </c>
+      <c r="A42" s="7"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+      <c r="A43" s="5">
+        <v>42457</v>
+      </c>
       <c r="B43" s="4"/>
       <c r="C43" s="3" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="A44" s="5"/>
       <c r="B44" s="4"/>
       <c r="C44" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="A45" s="5"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>42464</v>
-      </c>
+      <c r="A47" s="5"/>
       <c r="B47" s="4"/>
-      <c r="C47" s="3" t="s">
-        <v>37</v>
+      <c r="C47" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
+      <c r="A48" s="6"/>
       <c r="B48" s="4"/>
       <c r="C48" s="3" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="10"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
-        <v>42471</v>
-      </c>
+      <c r="A50" s="6"/>
       <c r="B50" s="4"/>
-      <c r="C50" s="3" t="s">
-        <v>40</v>
+      <c r="C50" s="13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A51" s="7"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="10"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="10"/>
+      <c r="A52" s="5">
+        <v>42464</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
-        <v>42478</v>
-      </c>
+      <c r="A53" s="5"/>
       <c r="B53" s="4"/>
       <c r="C53" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A54" s="7"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="10"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="10"/>
+      <c r="A55" s="5">
+        <v>42471</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
-        <v>42485</v>
-      </c>
+      <c r="A56" s="6"/>
       <c r="B56" s="4"/>
       <c r="C56" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="13" t="s">
-        <v>45</v>
-      </c>
+      <c r="A57" s="7"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
+      <c r="A58" s="5">
+        <v>42478</v>
+      </c>
       <c r="B58" s="4"/>
-      <c r="C58" s="13" t="s">
-        <v>44</v>
+      <c r="C58" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
+      <c r="A59" s="6"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
-        <v>42492</v>
-      </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="13" t="s">
-        <v>46</v>
-      </c>
+      <c r="A60" s="7"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="10"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
+      <c r="A61" s="5">
+        <v>42485</v>
+      </c>
       <c r="B61" s="4"/>
-      <c r="C61" s="13"/>
+      <c r="C61" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
@@ -1087,37 +1122,77 @@
       <c r="A63" s="6"/>
       <c r="B63" s="4"/>
       <c r="C63" s="13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="A64" s="7"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="10"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
+      <c r="A65" s="5">
+        <v>42492</v>
+      </c>
       <c r="B65" s="4"/>
       <c r="C65" s="13" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="4"/>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="13"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="10"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="10"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
màj planning 10/03 selon nouvelles instructions
</commit_message>
<xml_diff>
--- a/planning_stage.xlsx
+++ b/planning_stage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="120" windowWidth="23715" windowHeight="14325"/>
+    <workbookView xWindow="12210" yWindow="75" windowWidth="23715" windowHeight="14325"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>SEMAINE</t>
   </si>
@@ -129,12 +129,6 @@
     <t>Export (documentation) *.xlsx pour mesures instances (sélection, tout ou par critère)</t>
   </si>
   <si>
-    <t>Export IO et alarmes -&gt; *.xlsx pour une liste de sélection ou par critère</t>
-  </si>
-  <si>
-    <t>Débug export documentation</t>
-  </si>
-  <si>
     <t>Import/export -&gt; tests et débug complet</t>
   </si>
   <si>
@@ -147,15 +141,6 @@
     <t>? (Bouton d'aide -&gt; ouverture CHM)</t>
   </si>
   <si>
-    <t>? (Boite progression gérant annulation + numéro d'étape)</t>
-  </si>
-  <si>
-    <t>? (Raccourcis clavier (Ctrl+…) pour : recherche (F), refresh (U), layout (L))</t>
-  </si>
-  <si>
-    <t>Export (fonctionnel) de templates et instances : débug</t>
-  </si>
-  <si>
     <t>Possibilité de supprimer les UDAs des templates ou instances sélectionnés + confirm.</t>
   </si>
   <si>
@@ -165,6 +150,15 @@
     <t>Navigation depuis recherche: additionnée ou remplacement sélection</t>
   </si>
   <si>
+    <t>2j</t>
+  </si>
+  <si>
+    <t>3j</t>
+  </si>
+  <si>
+    <t>1j</t>
+  </si>
+  <si>
     <t>Import (fonctionnel) : debug</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>Boite de progression avec titre, numéro d'étape, croix d'annulation</t>
   </si>
   <si>
-    <t>Ajout export CSV à la manière d'ArchestrA</t>
-  </si>
-  <si>
     <t>Export (fonctionnel) de templates (par galaxie) et instances (par template) -&gt; XLSX</t>
   </si>
   <si>
@@ -199,13 +190,28 @@
   </si>
   <si>
     <t>UI Contrôleur d'export avec liste de sélection</t>
+  </si>
+  <si>
+    <t>Export IO -&gt; *.xlsx pour une liste de sélection ou par critère</t>
+  </si>
+  <si>
+    <t>Export alarmes -&gt; *.xlsx pour une liste de sélection ou par critère</t>
+  </si>
+  <si>
+    <t>Raccourcis clavier (Ctrl+…) pour : recherche (F), refresh (U), layout (L)</t>
+  </si>
+  <si>
+    <t>Export CSV à la manière d'ArchestrA</t>
+  </si>
+  <si>
+    <t>4j</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,13 +281,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -330,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -354,7 +353,6 @@
     <xf numFmtId="16" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,12 +781,12 @@
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="A15" s="14">
         <v>42436</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,14 +800,14 @@
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
       <c r="C17" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
       <c r="C18" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -844,35 +842,35 @@
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="4"/>
       <c r="C24" s="12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="12" t="s">
-        <v>56</v>
+      <c r="C25" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="4"/>
       <c r="C26" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,7 +882,9 @@
       <c r="A29" s="5">
         <v>42443</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C29" s="15" t="s">
         <v>25</v>
       </c>
@@ -913,64 +913,66 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="13" t="s">
+      <c r="B34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-    </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+      <c r="A36" s="7"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
         <v>42450</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="4"/>
       <c r="C37" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="3" t="s">
-        <v>55</v>
+      <c r="C38" s="15" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C40" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="A41" s="5"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -982,217 +984,282 @@
       <c r="A43" s="5">
         <v>42457</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="C43" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="4"/>
       <c r="C44" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="4"/>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="4"/>
       <c r="C48" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="5"/>
       <c r="B49" s="4"/>
       <c r="C49" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="A50" s="7"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="10"/>
+      <c r="A51" s="5">
+        <v>42464</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
-        <v>42464</v>
-      </c>
+      <c r="A52" s="5"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="C52" s="3"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="C53" s="3" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="10"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
-        <v>42471</v>
-      </c>
+      <c r="A55" s="5"/>
       <c r="B55" s="4"/>
       <c r="C55" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
+      <c r="A56" s="5"/>
       <c r="B56" s="4"/>
       <c r="C56" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="10"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>42471</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="10"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <v>42478</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="10"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>42485</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="10"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>42492</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
-        <v>42478</v>
-      </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="10"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <v>42485</v>
-      </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="3" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="13"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="13" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="13"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="10"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
-        <v>42492</v>
-      </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="13"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="10"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="7"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="10"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Màj planning 10/03 (selon changements instructions)
</commit_message>
<xml_diff>
--- a/planning_stage.xlsx
+++ b/planning_stage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>SEMAINE</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Recherches sur inclusion de styles en export *.docx</t>
   </si>
   <si>
-    <t>? (Lister tâches en attente, possibilité annuler, réordonner)</t>
-  </si>
-  <si>
     <t>Contrôleur d'instances (multi-colonnes triable et configurable)</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>Amélioration gestion de tâches et file d'attente</t>
   </si>
   <si>
-    <t>? (Bouton d'aide -&gt; ouverture CHM)</t>
-  </si>
-  <si>
     <t>Possibilité de supprimer les UDAs des templates ou instances sélectionnés + confirm.</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>Synchronisation des sélections d'arbres (depuis actif vers masqué)</t>
   </si>
   <si>
-    <t>? (Divers : stats (hôte,galax,nb tmpl) + nb inst chargées + nb total (sauf vues, …))</t>
-  </si>
-  <si>
     <t>UI Contrôleur d'export avec liste de sélection</t>
   </si>
   <si>
@@ -205,6 +196,12 @@
   </si>
   <si>
     <t>4j</t>
+  </si>
+  <si>
+    <t>? (Divers: Lister tâches en attente, possibilité annuler, réordonner)</t>
+  </si>
+  <si>
+    <t>? (Bouton d'aide (droite barre menu) -&gt; ouverture CHM)</t>
   </si>
 </sst>
 </file>
@@ -662,9 +659,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -737,42 +734,42 @@
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4"/>
       <c r="C11" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="4"/>
       <c r="C12" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="4"/>
       <c r="C13" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -786,91 +783,91 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="4"/>
       <c r="C16" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
       <c r="C17" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
       <c r="C18" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="4"/>
       <c r="C19" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="4"/>
       <c r="C20" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="4"/>
       <c r="C21" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="4"/>
       <c r="C22" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="4"/>
       <c r="C24" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="4"/>
       <c r="C25" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="4"/>
       <c r="C26" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -883,31 +880,31 @@
         <v>42443</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -918,17 +915,17 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="4"/>
       <c r="C35" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -941,17 +938,17 @@
         <v>42450</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="4"/>
       <c r="C38" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,17 +959,17 @@
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -985,31 +982,31 @@
         <v>42457</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="4"/>
       <c r="C44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="4"/>
       <c r="C45" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,10 +1017,10 @@
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1043,10 +1040,10 @@
         <v>42464</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,7 +1054,7 @@
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>10</v>
@@ -1074,14 +1071,14 @@
       <c r="A55" s="5"/>
       <c r="B55" s="4"/>
       <c r="C55" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="4"/>
       <c r="C56" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,10 +1098,10 @@
         <v>42471</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1115,10 +1112,10 @@
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1131,10 +1128,10 @@
         <v>42478</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1145,10 +1142,10 @@
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1161,10 +1158,10 @@
         <v>42485</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1175,10 +1172,10 @@
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1191,10 +1188,10 @@
         <v>42492</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1205,17 +1202,17 @@
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="4"/>
       <c r="C74" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,41 +1222,32 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
-      <c r="B76" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="B76" s="4"/>
       <c r="C76" s="13" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="4"/>
       <c r="C77" s="13" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="4"/>
       <c r="C78" s="13" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="A79" s="7"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="10"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="7"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="10"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
+      <c r="A80" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Images et màj planning semaine 07/03
</commit_message>
<xml_diff>
--- a/planning_stage.xlsx
+++ b/planning_stage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>SEMAINE</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Possibilité de supprimer les UDAs des templates ou instances sélectionnés + confirm.</t>
   </si>
   <si>
-    <t>? (Divers : supprimer instances sélectionnées)</t>
-  </si>
-  <si>
     <t>Navigation depuis recherche: additionnée ou remplacement sélection</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>Synchronisation des sélections d'arbres (depuis actif vers masqué)</t>
   </si>
   <si>
-    <t>UI Contrôleur d'export avec liste de sélection</t>
-  </si>
-  <si>
     <t>Export IO -&gt; *.xlsx pour une liste de sélection ou par critère</t>
   </si>
   <si>
@@ -202,6 +196,9 @@
   </si>
   <si>
     <t>? (Bouton d'aide (droite barre menu) -&gt; ouverture CHM)</t>
+  </si>
+  <si>
+    <t>UI Contrôleur d'export avec liste de sélection + UI contrôleur UDA</t>
   </si>
 </sst>
 </file>
@@ -659,9 +656,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -783,7 +780,7 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -797,14 +794,14 @@
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
       <c r="C17" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
       <c r="C18" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -839,35 +836,35 @@
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="4"/>
       <c r="C24" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="4"/>
       <c r="C25" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="4"/>
       <c r="C26" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="15" t="s">
-        <v>54</v>
+      <c r="C27" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,7 +877,7 @@
         <v>42443</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>24</v>
@@ -915,10 +912,10 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -938,17 +935,17 @@
         <v>42450</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="4"/>
       <c r="C38" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,7 +956,7 @@
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>27</v>
@@ -969,7 +966,7 @@
       <c r="A41" s="5"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -982,7 +979,7 @@
         <v>42457</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>28</v>
@@ -1006,7 +1003,7 @@
       <c r="A46" s="5"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,7 +1014,7 @@
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>14</v>
@@ -1040,7 +1037,7 @@
         <v>42464</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>39</v>
@@ -1054,7 +1051,7 @@
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>10</v>
@@ -1098,7 +1095,7 @@
         <v>42471</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>32</v>
@@ -1112,7 +1109,7 @@
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>35</v>
@@ -1128,7 +1125,7 @@
         <v>42478</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>35</v>
@@ -1142,10 +1139,10 @@
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1158,10 +1155,10 @@
         <v>42485</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1172,7 +1169,7 @@
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>36</v>
@@ -1188,7 +1185,7 @@
         <v>42492</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>37</v>
@@ -1202,10 +1199,10 @@
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1224,30 +1221,23 @@
       <c r="A76" s="6"/>
       <c r="B76" s="4"/>
       <c r="C76" s="13" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="4"/>
       <c r="C77" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="13" t="s">
-        <v>61</v>
-      </c>
+      <c r="A78" s="7"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="10"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
-      <c r="B79" s="9"/>
-      <c r="C79" s="10"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
+      <c r="A79" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Images, source et màj planning (semaine 14/03)
</commit_message>
<xml_diff>
--- a/planning_stage.xlsx
+++ b/planning_stage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>SEMAINE</t>
   </si>
@@ -99,12 +99,6 @@
     <t>Liste de sélection : drag n drop depuis arbre ou liste d'instances</t>
   </si>
   <si>
-    <t>Contrôleur d'import avec liste de validation + bouton retrait d'éléments</t>
-  </si>
-  <si>
-    <t>Liste validation affiche erreurs (ou boite de dialogue les mentionne)</t>
-  </si>
-  <si>
     <t>Importer de liste de validation vers GRAccess avec checkout, checkin ou undocheckout</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>Liste de sélection : ajout depuis arbre actif et liste d'inst (sélections) + éviter doublons</t>
   </si>
   <si>
-    <t>Contrôleur d'export spécial -&gt; tout, ou par critère (fonctionnel ou doc)</t>
-  </si>
-  <si>
     <t>Export (documentation) *.xlsx pour mesures instances (sélection, tout ou par critère)</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>Système de chargement/sauvegarde de snapshot d'état des arbres</t>
   </si>
   <si>
-    <t>Amélioration gestion de tâches et file d'attente</t>
-  </si>
-  <si>
     <t>Possibilité de supprimer les UDAs des templates ou instances sélectionnés + confirm.</t>
   </si>
   <si>
@@ -150,9 +138,6 @@
     <t>1j</t>
   </si>
   <si>
-    <t>Import (fonctionnel) : debug</t>
-  </si>
-  <si>
     <t>Optimisation récupération et vitesse affichage (de 16 sec à 1 sec)</t>
   </si>
   <si>
@@ -162,9 +147,6 @@
     <t>Boite de progression avec titre, numéro d'étape, croix d'annulation</t>
   </si>
   <si>
-    <t>Export (fonctionnel) de templates (par galaxie) et instances (par template) -&gt; XLSX</t>
-  </si>
-  <si>
     <t>Import (fonctionnel) d'instances (par template) ou tmpl depuis XLSX vers liste</t>
   </si>
   <si>
@@ -199,6 +181,39 @@
   </si>
   <si>
     <t>UI Contrôleur d'export avec liste de sélection + UI contrôleur UDA</t>
+  </si>
+  <si>
+    <t>5j</t>
+  </si>
+  <si>
+    <t>Contrôleur d'export par catégorie (tout ou par critère)</t>
+  </si>
+  <si>
+    <t>Récupération SQL d'éléments par catégorie/critère</t>
+  </si>
+  <si>
+    <t>Obtenir détails et attributs/UDAs pour export fonctionnel</t>
+  </si>
+  <si>
+    <t>Export fonctionnel de templates/instances (par template) -&gt; XLSX</t>
+  </si>
+  <si>
+    <t>Debug de l'export fonctionnel de templates/instances</t>
+  </si>
+  <si>
+    <t>Export fonctionnel - onglet général avec infos + liste templates + listes valeurs possibles</t>
+  </si>
+  <si>
+    <t>Export fonctionnel - décompte dynamique du nombre de templates/instances</t>
+  </si>
+  <si>
+    <t>Export fonctionnel - un onglet par template + gérer UDAs + interprétation arrays</t>
+  </si>
+  <si>
+    <t>Contrôleur d'import avec liste de validation + bouton retrait + gestion erreurs</t>
+  </si>
+  <si>
+    <t>Debug de l'import/export fonctionnel de templates/instances</t>
   </si>
 </sst>
 </file>
@@ -656,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +795,7 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -794,14 +809,14 @@
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
       <c r="C17" s="12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
       <c r="C18" s="12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,275 +829,263 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="4"/>
       <c r="C21" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="4"/>
       <c r="C22" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="12" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="4"/>
       <c r="C24" s="12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="16" t="s">
-        <v>50</v>
+      <c r="C25" s="12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="4"/>
       <c r="C26" s="16" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="12" t="s">
-        <v>60</v>
-      </c>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="16" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
         <v>42443</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="15" t="s">
-        <v>33</v>
+      <c r="C31" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="15" t="s">
-        <v>25</v>
+      <c r="C32" s="16" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="15"/>
+      <c r="C33" s="16"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>48</v>
+      <c r="B34" s="4"/>
+      <c r="C34" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="13" t="s">
-        <v>26</v>
+      <c r="C35" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="6"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
         <v>42450</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>42457</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="3"/>
+      <c r="B47" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="B48" s="4"/>
       <c r="C48" s="3" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="4"/>
       <c r="C49" s="3" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="10"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
-        <v>42464</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>39</v>
+      <c r="A51" s="5"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="3"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
+      <c r="A53" s="5">
+        <v>42457</v>
+      </c>
       <c r="B53" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="3" t="s">
-        <v>9</v>
+      <c r="C54" s="15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="4"/>
-      <c r="C55" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="C55" s="15"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
-      <c r="B56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C56" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="4"/>
       <c r="C57" s="13" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1092,152 +1095,182 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>42471</v>
+        <v>42464</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="4"/>
-      <c r="C60" s="3"/>
+      <c r="C60" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="A61" s="5"/>
+      <c r="B61" s="4"/>
       <c r="C61" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="10"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
-        <v>42478</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="A63" s="7"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="10"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="3"/>
+      <c r="A64" s="5">
+        <v>42471</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
-      <c r="B65" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="3"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="10"/>
+      <c r="A66" s="6"/>
+      <c r="B66" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
-        <v>42485</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="A67" s="7"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="10"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="3"/>
+      <c r="A68" s="5">
+        <v>42478</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
-      <c r="B69" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="B69" s="4"/>
+      <c r="C69" s="3"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="10"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
-        <v>42492</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>37</v>
-      </c>
+      <c r="A71" s="7"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="13"/>
+      <c r="A72" s="5">
+        <v>42485</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
-      <c r="B73" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>55</v>
-      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="3"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="13" t="s">
-        <v>38</v>
+      <c r="B74" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="13"/>
+      <c r="A75" s="7"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="5">
+        <v>42492</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C76" s="13" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
+      <c r="A77" s="5"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="C77" s="13"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="7"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="10"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
+      <c r="A79" s="6"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="13"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="7"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="10"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mise à jour semaine 18/04
</commit_message>
<xml_diff>
--- a/planning_stage.xlsx
+++ b/planning_stage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="35460" yWindow="75" windowWidth="23715" windowHeight="14325"/>
+    <workbookView xWindow="36390" yWindow="75" windowWidth="23715" windowHeight="14325"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>Export de type ArchestrA - base</t>
   </si>
   <si>
-    <t>Export de type ArchestrA - suite</t>
-  </si>
-  <si>
     <t>Export (documentation) *.xlsx pour mesures instances</t>
   </si>
   <si>
@@ -228,13 +225,16 @@
   </si>
   <si>
     <t>Tests utilisateurs/ergonomie + tests performances</t>
+  </si>
+  <si>
+    <t>Export de type ArchestrA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +296,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -344,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -369,6 +376,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1229,14 +1237,14 @@
       <c r="A78" s="5"/>
       <c r="B78" s="15"/>
       <c r="C78" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="4"/>
       <c r="C79" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,12 +1253,12 @@
       <c r="C80" s="10"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="5">
+      <c r="A81" s="16">
         <v>42478</v>
       </c>
       <c r="B81" s="4"/>
-      <c r="C81" s="3" t="s">
-        <v>64</v>
+      <c r="C81" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,7 +1272,7 @@
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1278,14 +1286,14 @@
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
semaine 25/04 + tests perfs
</commit_message>
<xml_diff>
--- a/planning_stage.xlsx
+++ b/planning_stage.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lumar\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="40110" yWindow="75" windowWidth="23715" windowHeight="14325"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>SEMAINE</t>
   </si>
@@ -221,9 +216,6 @@
     <t>Export (documentation) *.xlsx pour alarmes instances</t>
   </si>
   <si>
-    <t>Tests avancés/debug final</t>
-  </si>
-  <si>
     <t>Export de type ArchestrA</t>
   </si>
   <si>
@@ -233,13 +225,22 @@
     <t>Drag and drop depuis liste instances</t>
   </si>
   <si>
-    <t>Tests performances + tests utilisateurs</t>
-  </si>
-  <si>
     <t>Sauvegarde paramètres connexion dans registre</t>
   </si>
   <si>
     <t>Aspect visuel amélioré</t>
+  </si>
+  <si>
+    <t>Tests performances</t>
+  </si>
+  <si>
+    <t>Tests utilisateurs</t>
+  </si>
+  <si>
+    <t>About box + assembly info</t>
+  </si>
+  <si>
+    <t>Améliorations UX (autoscroll lors de navigation depuis recherche, tooltips, …)</t>
   </si>
 </sst>
 </file>
@@ -454,7 +455,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,7 +490,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -698,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,21 +1271,21 @@
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
       <c r="B82" s="4"/>
       <c r="C82" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="16"/>
       <c r="B83" s="4"/>
       <c r="C83" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1293,49 +1294,68 @@
       <c r="C84" s="10"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
+      <c r="A85" s="13">
         <v>42485</v>
       </c>
       <c r="B85" s="4"/>
-      <c r="C85" s="3" t="s">
-        <v>70</v>
+      <c r="C85" s="12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="4"/>
       <c r="C86" s="12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="4"/>
       <c r="C87" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="7"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="10"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="12" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
+      <c r="A89" s="5"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="7"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="10"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
         <v>42492</v>
       </c>
-      <c r="B89" s="4"/>
-      <c r="C89" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="7"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="7"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="10"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>